<commit_message>
Added changes for Security Config
</commit_message>
<xml_diff>
--- a/src/main/resources/static/assets/patients.xlsx
+++ b/src/main/resources/static/assets/patients.xlsx
@@ -1,45 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheela\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09F2BA1-A9F4-4232-89F4-F73C2C17F71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48690018-C2B3-4B8F-9C63-C8DB0162F21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Patients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>dignosis</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>patient_name</t>
-  </si>
-  <si>
-    <t>symptoms</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
   </si>
   <si>
     <t>abc</t>
@@ -49,6 +47,9 @@
   </si>
   <si>
     <t>abcde</t>
+  </si>
+  <si>
+    <t>2024-04-03</t>
   </si>
   <si>
     <t>niki</t>
@@ -70,7 +71,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,7 +134,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -145,7 +146,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -192,6 +193,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -227,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,26 +417,27 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -414,51 +450,51 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>45384</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>45385</v>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>45385</v>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added changes in patientRecord file
</commit_message>
<xml_diff>
--- a/src/main/resources/static/assets/patients.xlsx
+++ b/src/main/resources/static/assets/patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheela\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48690018-C2B3-4B8F-9C63-C8DB0162F21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654DCC1-791C-4500-8414-8DD209914208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,13 +417,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.77734375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
@@ -499,5 +499,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>